<commit_message>
update: new generic pipeline
</commit_message>
<xml_diff>
--- a/experiments/miliane-CxAC-trim/sheets/abundance-ranks-miliane-CxAC-trim.xlsx
+++ b/experiments/miliane-CxAC-trim/sheets/abundance-ranks-miliane-CxAC-trim.xlsx
@@ -197,12 +197,12 @@
     <t>Christensenellales</t>
   </si>
   <si>
+    <t>Sphingobacteriales</t>
+  </si>
+  <si>
     <t>Micrococcales</t>
   </si>
   <si>
-    <t>Sphingobacteriales</t>
-  </si>
-  <si>
     <t>RF39</t>
   </si>
   <si>
@@ -473,12 +473,12 @@
     <t>[Eubacterium]_nodatum_group</t>
   </si>
   <si>
+    <t>Streptococcus</t>
+  </si>
+  <si>
     <t>Enhydrobacter</t>
   </si>
   <si>
-    <t>Streptococcus</t>
-  </si>
-  <si>
     <t>Pantoea</t>
   </si>
   <si>
@@ -518,16 +518,16 @@
     <t>Enterococcus</t>
   </si>
   <si>
+    <t>Veillonella</t>
+  </si>
+  <si>
     <t>Erysipelatoclostridium</t>
   </si>
   <si>
-    <t>Veillonella</t>
+    <t>Aquabacterium</t>
   </si>
   <si>
     <t>Brevundimonas</t>
-  </si>
-  <si>
-    <t>Aquabacterium</t>
   </si>
   <si>
     <t>Aerococcus</t>
@@ -27696,10 +27696,10 @@
         <v>74</v>
       </c>
       <c r="C22">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -27717,7 +27717,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -27732,10 +27732,10 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="P22">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -27746,10 +27746,10 @@
         <v>74</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D23">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -27767,7 +27767,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -27782,10 +27782,10 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -33066,10 +33066,10 @@
         <v>97</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D50">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -33084,7 +33084,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -33105,7 +33105,7 @@
         <v>0</v>
       </c>
       <c r="P50">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -33116,10 +33116,10 @@
         <v>97</v>
       </c>
       <c r="C51">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -33134,7 +33134,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -33155,7 +33155,7 @@
         <v>0</v>
       </c>
       <c r="P51">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -33896,16 +33896,16 @@
         <v>0</v>
       </c>
       <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
         <v>10</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <v>0</v>
-      </c>
-      <c r="P66">
-        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -33946,7 +33946,7 @@
         <v>0</v>
       </c>
       <c r="M67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -33955,7 +33955,7 @@
         <v>0</v>
       </c>
       <c r="P67">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -33993,7 +33993,7 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M68">
         <v>0</v>
@@ -34002,7 +34002,7 @@
         <v>0</v>
       </c>
       <c r="O68">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P68">
         <v>0</v>
@@ -34043,16 +34043,16 @@
         <v>0</v>
       </c>
       <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
         <v>8</v>
-      </c>
-      <c r="M69">
-        <v>0</v>
-      </c>
-      <c r="N69">
-        <v>0</v>
-      </c>
-      <c r="O69">
-        <v>0</v>
       </c>
       <c r="P69">
         <v>0</v>

</xml_diff>